<commit_message>
Deploying to gh-pages from  @ 04521bd8d823bbb6ba65e2b0c0c23896a7acf049 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2023_5-3-2.xlsx
+++ b/assets/excel/2023_5-3-2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15_Uebergreifende_Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB38C653-2067-4F63-9665-7765AE42F8EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6589D8C-BD23-4992-8EF6-074EE701A7C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{73340D0E-D62F-4D83-B33C-29358B8E4782}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" xr2:uid="{73340D0E-D62F-4D83-B33C-29358B8E4782}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,27 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
-    <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2022</t>
-  </si>
-  <si>
     <t>Indikator 5.3.2: Entwicklung der Arbeitslosenquote in Niedersachsen</t>
   </si>
   <si>
     <t>Tabelle 5.3.2: Entwicklung der Arbeitslosenquoten nach Staatsangehörikeit und Geschlecht in Niedersachsen</t>
-  </si>
-  <si>
-    <r>
-      <t>Berichtsmonat</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="6"/>
-        <color indexed="8"/>
-        <rFont val="NDSFrutiger 45 Light"/>
-      </rPr>
-      <t>1)</t>
-    </r>
   </si>
   <si>
     <t>Arbeitslosenquote Insgesamt
@@ -106,6 +89,12 @@
   </si>
   <si>
     <t>https://www.integrationsmonitoring.niedersachsen.de</t>
+  </si>
+  <si>
+    <t>Berichtsmonat</t>
+  </si>
+  <si>
+    <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2023</t>
   </si>
 </sst>
 </file>
@@ -117,7 +106,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="\+0.0;\-0.0;0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,12 +131,6 @@
       <name val="NDSFrutiger 55 Roman"/>
     </font>
     <font>
-      <sz val="6"/>
-      <color indexed="8"/>
-      <name val="NDSFrutiger 45 Light"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="6"/>
       <color indexed="8"/>
       <name val="NDSFrutiger 45 Light"/>
@@ -183,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -277,35 +260,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color indexed="22"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color indexed="22"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -316,106 +270,100 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -738,1269 +686,1269 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:T33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+    </row>
+    <row r="4" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="6" spans="2:20" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="6" spans="2:20" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
+      <c r="J6" s="21"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7" t="s">
+      <c r="M6" s="19"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8" t="s">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="8" t="s">
+      <c r="S6" s="21"/>
+      <c r="T6" s="18"/>
+    </row>
+    <row r="7" spans="2:20" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="28"/>
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="8"/>
-    </row>
-    <row r="7" spans="2:20" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
+      <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="H7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="N7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="29"/>
+      <c r="C8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="24"/>
+      <c r="T8" s="22"/>
+    </row>
+    <row r="9" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7">
+        <v>4</v>
+      </c>
+      <c r="F9" s="7">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7">
+        <v>6</v>
+      </c>
+      <c r="H9" s="7">
+        <v>7</v>
+      </c>
+      <c r="I9" s="7">
+        <v>8</v>
+      </c>
+      <c r="J9" s="7">
+        <v>9</v>
+      </c>
+      <c r="K9" s="7">
         <v>10</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="L9" s="7">
+        <v>11</v>
+      </c>
+      <c r="M9" s="7">
+        <v>12</v>
+      </c>
+      <c r="N9" s="7">
         <v>13</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="11" t="s">
+      <c r="O9" s="7">
+        <v>14</v>
+      </c>
+      <c r="P9" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="30">
+        <v>39263</v>
+      </c>
+      <c r="C10" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="D10" s="8">
+        <v>7.8</v>
+      </c>
+      <c r="E10" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F10" s="8">
+        <v>21.1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>18.8</v>
+      </c>
+      <c r="H10" s="8">
+        <v>24.4</v>
+      </c>
+      <c r="I10" s="9">
+        <v>12.600000000000001</v>
+      </c>
+      <c r="J10" s="9">
         <v>11</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="C8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="S8" s="17"/>
-      <c r="T8" s="15"/>
-    </row>
-    <row r="9" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19">
-        <v>1</v>
-      </c>
-      <c r="C9" s="19">
-        <v>2</v>
-      </c>
-      <c r="D9" s="19">
-        <v>3</v>
-      </c>
-      <c r="E9" s="19">
-        <v>4</v>
-      </c>
-      <c r="F9" s="19">
-        <v>5</v>
-      </c>
-      <c r="G9" s="19">
-        <v>6</v>
-      </c>
-      <c r="H9" s="19">
-        <v>7</v>
-      </c>
-      <c r="I9" s="19">
-        <v>8</v>
-      </c>
-      <c r="J9" s="19">
-        <v>9</v>
-      </c>
-      <c r="K9" s="19">
-        <v>10</v>
-      </c>
-      <c r="L9" s="19">
-        <v>11</v>
-      </c>
-      <c r="M9" s="19">
-        <v>12</v>
-      </c>
-      <c r="N9" s="19">
-        <v>13</v>
-      </c>
-      <c r="O9" s="19">
-        <v>14</v>
-      </c>
-      <c r="P9" s="19">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="19">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="29">
-        <v>39263</v>
-      </c>
-      <c r="C10" s="20">
-        <v>8.5</v>
-      </c>
-      <c r="D10" s="20">
-        <v>7.8</v>
-      </c>
-      <c r="E10" s="20">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="F10" s="20">
-        <v>21.1</v>
-      </c>
-      <c r="G10" s="20">
-        <v>18.8</v>
-      </c>
-      <c r="H10" s="20">
-        <v>24.4</v>
-      </c>
-      <c r="I10" s="21">
-        <v>12.600000000000001</v>
-      </c>
-      <c r="J10" s="21">
-        <v>11</v>
-      </c>
-      <c r="K10" s="21">
+      <c r="K10" s="9">
         <v>15.2</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="10">
         <v>7.9</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="10">
         <v>4.7</v>
       </c>
-      <c r="N10" s="22">
+      <c r="N10" s="10">
         <v>9.3000000000000007</v>
       </c>
-      <c r="O10" s="22">
+      <c r="O10" s="10">
         <v>15.3</v>
       </c>
-      <c r="P10" s="22">
+      <c r="P10" s="10">
         <v>14.2</v>
       </c>
-      <c r="Q10" s="22">
+      <c r="Q10" s="10">
         <v>15.6</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="11">
         <v>7.4</v>
       </c>
-      <c r="S10" s="23">
+      <c r="S10" s="11">
         <v>9.5</v>
       </c>
-      <c r="T10" s="23">
+      <c r="T10" s="11">
         <v>6.2999999999999989</v>
       </c>
     </row>
-    <row r="11" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="30">
         <v>39629</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="8">
         <v>7.4</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="8">
         <v>6.9</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="8">
         <v>7.9</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="8">
         <v>20</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="8">
         <v>17.5</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="8">
         <v>23.6</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="9">
         <v>12.6</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="9">
         <v>10.6</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="9">
         <v>15.700000000000001</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="10">
         <v>6.3</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="10">
         <v>3.5</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="10">
         <v>7.5</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="10">
         <v>13.5</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="10">
         <v>12</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="10">
         <v>14.1</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="11">
         <v>7.2</v>
       </c>
-      <c r="S11" s="23">
+      <c r="S11" s="11">
         <v>8.5</v>
       </c>
-      <c r="T11" s="23">
+      <c r="T11" s="11">
         <v>6.6</v>
       </c>
     </row>
-    <row r="12" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="30">
         <v>39994</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="8">
         <v>7.6</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="8">
         <v>7.7</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="8">
         <v>7.5</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="8">
         <v>19.8</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="8">
         <v>18.3</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="8">
         <v>21.8</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="9">
         <v>12.200000000000001</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="9">
         <v>10.600000000000001</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="9">
         <v>14.3</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="10">
         <v>7.4</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="10">
         <v>3.7</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="10">
         <v>9</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="10">
         <v>14</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="10">
         <v>10.7</v>
       </c>
-      <c r="Q12" s="22">
+      <c r="Q12" s="10">
         <v>15.2</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="11">
         <v>6.6</v>
       </c>
-      <c r="S12" s="23">
+      <c r="S12" s="11">
         <v>6.9999999999999991</v>
       </c>
-      <c r="T12" s="23">
+      <c r="T12" s="11">
         <v>6.1999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="30">
         <v>40359</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="8">
         <v>7.3</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="8">
         <v>7.3</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="8">
         <v>7.3</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="8">
         <v>18.5</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="8">
         <v>16.899999999999999</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="8">
         <v>20.6</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="9">
         <v>11.2</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="9">
         <v>9.5999999999999979</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="9">
         <v>13.3</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="10">
         <v>6.6</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="10">
         <v>3.5</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="10">
         <v>8</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="10">
         <v>13</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="10">
         <v>10.5</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="10">
         <v>13.9</v>
       </c>
-      <c r="R13" s="23">
+      <c r="R13" s="11">
         <v>6.4</v>
       </c>
-      <c r="S13" s="23">
+      <c r="S13" s="11">
         <v>7</v>
       </c>
-      <c r="T13" s="23">
+      <c r="T13" s="11">
         <v>5.9</v>
       </c>
     </row>
-    <row r="14" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="30">
         <v>40724</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="8">
         <v>6.7</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="8">
         <v>6.5</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="8">
         <v>6.9</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="8">
         <v>17.399999999999999</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="8">
         <v>15.7</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="8">
         <v>19.7</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="9">
         <v>10.7</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="9">
         <v>9.1999999999999993</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="9">
         <v>12.799999999999999</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="10">
         <v>5.4</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="10">
         <v>2.9</v>
       </c>
-      <c r="N14" s="22">
+      <c r="N14" s="10">
         <v>6.5</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="10">
         <v>12</v>
       </c>
-      <c r="P14" s="22">
+      <c r="P14" s="10">
         <v>9.4</v>
       </c>
-      <c r="Q14" s="22">
+      <c r="Q14" s="10">
         <v>12.9</v>
       </c>
-      <c r="R14" s="23">
+      <c r="R14" s="11">
         <v>6.6</v>
       </c>
-      <c r="S14" s="23">
+      <c r="S14" s="11">
         <v>6.5</v>
       </c>
-      <c r="T14" s="23">
+      <c r="T14" s="11">
         <v>6.4</v>
       </c>
     </row>
-    <row r="15" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="30">
         <v>41090</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="8">
         <v>6.2</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="8">
         <v>6.1</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="8">
         <v>6.4</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="8">
         <v>16.2</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="8">
         <v>14.5</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="8">
         <v>18.5</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="9">
         <v>10</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="9">
         <v>8.4</v>
       </c>
-      <c r="K15" s="21">
+      <c r="K15" s="9">
         <v>12.1</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="10">
         <v>5.2</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="10">
         <v>3</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="10">
         <v>6.1</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="10">
         <v>11.3</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="10">
         <v>8.8000000000000007</v>
       </c>
-      <c r="Q15" s="22">
+      <c r="Q15" s="10">
         <v>12.2</v>
       </c>
-      <c r="R15" s="23">
+      <c r="R15" s="11">
         <v>6.1000000000000005</v>
       </c>
-      <c r="S15" s="23">
+      <c r="S15" s="11">
         <v>5.8000000000000007</v>
       </c>
-      <c r="T15" s="23">
+      <c r="T15" s="11">
         <v>6.1</v>
       </c>
     </row>
-    <row r="16" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="30">
         <v>41455</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="8">
         <v>6.3</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="8">
         <v>6.3</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="8">
         <v>6.4</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="8">
         <v>15.9</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="8">
         <v>14.3</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="8">
         <v>18.2</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="9">
         <v>9.6000000000000014</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="9">
         <v>8</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="9">
         <v>11.799999999999999</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="10">
         <v>5.7</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="10">
         <v>3.1</v>
       </c>
-      <c r="N16" s="22">
+      <c r="N16" s="10">
         <v>6.7</v>
       </c>
-      <c r="O16" s="22">
+      <c r="O16" s="10">
         <v>11.3</v>
       </c>
-      <c r="P16" s="22">
+      <c r="P16" s="10">
         <v>9.6</v>
       </c>
-      <c r="Q16" s="22">
+      <c r="Q16" s="10">
         <v>11.8</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="11">
         <v>5.6000000000000005</v>
       </c>
-      <c r="S16" s="23">
+      <c r="S16" s="11">
         <v>6.5</v>
       </c>
-      <c r="T16" s="23">
+      <c r="T16" s="11">
         <v>5.1000000000000005</v>
       </c>
     </row>
-    <row r="17" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="30">
         <v>41820</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="8">
         <v>6.3</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="8">
         <v>6.3</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="8">
         <v>6.3</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="8">
         <v>16.2</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="8">
         <v>14.4</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="8">
         <v>18.8</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="9">
         <v>9.8999999999999986</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="9">
         <v>8.1000000000000014</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="9">
         <v>12.5</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="10">
         <v>5.3</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="10">
         <v>3</v>
       </c>
-      <c r="N17" s="22">
+      <c r="N17" s="10">
         <v>6.2</v>
       </c>
-      <c r="O17" s="22">
+      <c r="O17" s="10">
         <v>12.1</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="10">
         <v>10.8</v>
       </c>
-      <c r="Q17" s="22">
+      <c r="Q17" s="10">
         <v>12.4</v>
       </c>
-      <c r="R17" s="23">
+      <c r="R17" s="11">
         <v>6.8</v>
       </c>
-      <c r="S17" s="23">
+      <c r="S17" s="11">
         <v>7.8000000000000007</v>
       </c>
-      <c r="T17" s="23">
+      <c r="T17" s="11">
         <v>6.2</v>
       </c>
     </row>
-    <row r="18" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="30">
         <v>42185</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="8">
         <v>5.9</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="8">
         <v>5.9</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="8">
         <v>5.8</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="8">
         <v>16.600000000000001</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="8">
         <v>14.6</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="8">
         <v>19.399999999999999</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="9">
         <v>10.700000000000001</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="9">
         <v>8.6999999999999993</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="9">
         <v>13.599999999999998</v>
       </c>
-      <c r="L18" s="22">
+      <c r="L18" s="10">
         <v>4.8</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="10">
         <v>2.9</v>
       </c>
-      <c r="N18" s="22">
+      <c r="N18" s="10">
         <v>5.6</v>
       </c>
-      <c r="O18" s="22">
+      <c r="O18" s="10">
         <v>12.4</v>
       </c>
-      <c r="P18" s="22">
+      <c r="P18" s="10">
         <v>12.2</v>
       </c>
-      <c r="Q18" s="22">
+      <c r="Q18" s="10">
         <v>12.4</v>
       </c>
-      <c r="R18" s="23">
+      <c r="R18" s="11">
         <v>7.6000000000000005</v>
       </c>
-      <c r="S18" s="23">
+      <c r="S18" s="11">
         <v>9.2999999999999989</v>
       </c>
-      <c r="T18" s="23">
+      <c r="T18" s="11">
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="19" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="30">
         <v>42551</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="8">
         <v>5.8</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="8">
         <v>6</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="8">
         <v>5.6</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="8">
         <v>18.399999999999999</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="8">
         <v>17.600000000000001</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="8">
         <v>19.5</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="9">
         <v>12.599999999999998</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="9">
         <v>11.600000000000001</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="9">
         <v>13.9</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="10">
         <v>5.6</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="10">
         <v>3.4</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="10">
         <v>6.6</v>
       </c>
-      <c r="O19" s="22">
+      <c r="O19" s="10">
         <v>18.7</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P19" s="10">
         <v>16.899999999999999</v>
       </c>
-      <c r="Q19" s="22">
+      <c r="Q19" s="10">
         <v>19.2</v>
       </c>
-      <c r="R19" s="23">
+      <c r="R19" s="11">
         <v>13.1</v>
       </c>
-      <c r="S19" s="23">
+      <c r="S19" s="11">
         <v>13.499999999999998</v>
       </c>
-      <c r="T19" s="23">
+      <c r="T19" s="11">
         <v>12.6</v>
       </c>
     </row>
-    <row r="20" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="30">
         <v>42916</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="8">
         <v>5.6</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="8">
         <v>5.8</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="8">
         <v>5.5</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="8">
         <v>17.899999999999999</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="8">
         <v>16.5</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H20" s="8">
         <v>20</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="9">
         <v>12.299999999999999</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="9">
         <v>10.7</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="9">
         <v>14.5</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="10">
         <v>5.3</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="10">
         <v>3.1</v>
       </c>
-      <c r="N20" s="22">
+      <c r="N20" s="10">
         <v>6.3</v>
       </c>
-      <c r="O20" s="22">
+      <c r="O20" s="10">
         <v>16.600000000000001</v>
       </c>
-      <c r="P20" s="22">
+      <c r="P20" s="10">
         <v>13.6</v>
       </c>
-      <c r="Q20" s="22">
+      <c r="Q20" s="10">
         <v>17.5</v>
       </c>
-      <c r="R20" s="23">
+      <c r="R20" s="11">
         <v>11.3</v>
       </c>
-      <c r="S20" s="23">
+      <c r="S20" s="11">
         <v>10.5</v>
       </c>
-      <c r="T20" s="23">
+      <c r="T20" s="11">
         <v>11.2</v>
       </c>
     </row>
-    <row r="21" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="30">
         <v>43281</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="8">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="8">
         <v>5.3</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="8">
         <v>5</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="8">
         <v>15.9</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="8">
         <v>14.4</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="8">
         <v>18.2</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="9">
         <v>10.8</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="9">
         <v>9.1000000000000014</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K21" s="9">
         <v>13.2</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="10">
         <v>4.7</v>
       </c>
-      <c r="M21" s="22">
+      <c r="M21" s="10">
         <v>2.9</v>
       </c>
-      <c r="N21" s="22">
+      <c r="N21" s="10">
         <v>5.5</v>
       </c>
-      <c r="O21" s="22">
+      <c r="O21" s="10">
         <v>13.8</v>
       </c>
-      <c r="P21" s="22">
+      <c r="P21" s="10">
         <v>11.6</v>
       </c>
-      <c r="Q21" s="22">
+      <c r="Q21" s="10">
         <v>14.3</v>
       </c>
-      <c r="R21" s="23">
+      <c r="R21" s="11">
         <v>9.1000000000000014</v>
       </c>
-      <c r="S21" s="23">
+      <c r="S21" s="11">
         <v>8.6999999999999993</v>
       </c>
-      <c r="T21" s="23">
+      <c r="T21" s="11">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="22" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="30">
         <v>43646</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="8">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="8">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="8">
         <v>4.7</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="8">
         <v>15</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="8">
         <v>13.5</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="8">
         <v>17.399999999999999</v>
       </c>
-      <c r="I22" s="21">
+      <c r="I22" s="9">
         <v>10.1</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="9">
         <v>8.4</v>
       </c>
-      <c r="K22" s="21">
+      <c r="K22" s="9">
         <v>12.7</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="10">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="10">
         <v>2.6</v>
       </c>
-      <c r="N22" s="22">
+      <c r="N22" s="10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="O22" s="22">
+      <c r="O22" s="10">
         <v>12.3</v>
       </c>
-      <c r="P22" s="22">
+      <c r="P22" s="10">
         <v>9.6</v>
       </c>
-      <c r="Q22" s="22">
+      <c r="Q22" s="10">
         <v>13</v>
       </c>
-      <c r="R22" s="23">
+      <c r="R22" s="11">
         <v>7.9</v>
       </c>
-      <c r="S22" s="23">
+      <c r="S22" s="11">
         <v>7</v>
       </c>
-      <c r="T22" s="23">
+      <c r="T22" s="11">
         <v>7.9</v>
       </c>
     </row>
-    <row r="23" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="30">
         <v>44012</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="8">
         <v>6</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="8">
         <v>6.4</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="8">
         <v>5.7</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="8">
         <v>18.100000000000001</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="8">
         <v>16.5</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="8">
         <v>20.6</v>
       </c>
-      <c r="I23" s="21">
+      <c r="I23" s="9">
         <v>12.100000000000001</v>
       </c>
-      <c r="J23" s="21">
+      <c r="J23" s="9">
         <v>10.1</v>
       </c>
-      <c r="K23" s="21">
+      <c r="K23" s="9">
         <v>14.900000000000002</v>
       </c>
-      <c r="L23" s="22">
+      <c r="L23" s="10">
         <v>6</v>
       </c>
-      <c r="M23" s="22">
+      <c r="M23" s="10">
         <v>3.4</v>
       </c>
-      <c r="N23" s="22">
+      <c r="N23" s="10">
         <v>7.1</v>
       </c>
-      <c r="O23" s="22">
+      <c r="O23" s="10">
         <v>15.2</v>
       </c>
-      <c r="P23" s="22">
+      <c r="P23" s="10">
         <v>11.4</v>
       </c>
-      <c r="Q23" s="22">
+      <c r="Q23" s="10">
         <v>16.100000000000001</v>
       </c>
-      <c r="R23" s="23">
+      <c r="R23" s="11">
         <v>9.1999999999999993</v>
       </c>
-      <c r="S23" s="23">
+      <c r="S23" s="11">
         <v>8</v>
       </c>
-      <c r="T23" s="23">
+      <c r="T23" s="11">
         <v>9.0000000000000018</v>
       </c>
     </row>
-    <row r="24" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="30">
         <v>44377</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="8">
         <v>5.5</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="8">
         <v>5.7</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="8">
         <v>5.3</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="8">
         <v>15.9</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="8">
         <v>13.9</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="8">
         <v>19.3</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I24" s="9">
         <v>10.4</v>
       </c>
-      <c r="J24" s="21">
+      <c r="J24" s="9">
         <v>8.1999999999999993</v>
       </c>
-      <c r="K24" s="21">
+      <c r="K24" s="9">
         <v>14</v>
       </c>
-      <c r="L24" s="22">
+      <c r="L24" s="10">
         <v>4.7</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M24" s="10">
         <v>2.7</v>
       </c>
-      <c r="N24" s="22">
+      <c r="N24" s="10">
         <v>5.4</v>
       </c>
-      <c r="O24" s="22">
+      <c r="O24" s="10">
         <v>11.7</v>
       </c>
-      <c r="P24" s="22">
+      <c r="P24" s="10">
         <v>10.4</v>
       </c>
-      <c r="Q24" s="22">
+      <c r="Q24" s="10">
         <v>11.9</v>
       </c>
-      <c r="R24" s="23">
+      <c r="R24" s="11">
         <v>6.9999999999999991</v>
       </c>
-      <c r="S24" s="23">
+      <c r="S24" s="11">
         <v>7.7</v>
       </c>
-      <c r="T24" s="23">
+      <c r="T24" s="11">
         <v>6.5</v>
       </c>
     </row>
-    <row r="25" spans="2:20" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:20" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="30">
         <v>44742</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="8">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="8">
         <v>5.2</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="8">
         <v>5</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="8">
         <v>16.399999999999999</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="8">
         <v>12.8</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="8">
         <v>22</v>
       </c>
-      <c r="I25" s="21">
+      <c r="I25" s="9">
         <v>11.299999999999999</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J25" s="9">
         <v>7.6000000000000005</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="9">
         <v>17</v>
       </c>
-      <c r="L25" s="22">
+      <c r="L25" s="10">
         <v>4.2</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="10">
         <v>3.2</v>
       </c>
-      <c r="N25" s="22">
+      <c r="N25" s="10">
         <v>4.5999999999999996</v>
       </c>
-      <c r="O25" s="22">
+      <c r="O25" s="10">
         <v>12.8</v>
       </c>
-      <c r="P25" s="22">
+      <c r="P25" s="10">
         <v>18.2</v>
       </c>
-      <c r="Q25" s="22">
+      <c r="Q25" s="10">
         <v>11.7</v>
       </c>
-      <c r="R25" s="23">
+      <c r="R25" s="11">
         <v>8.6000000000000014</v>
       </c>
-      <c r="S25" s="23">
+      <c r="S25" s="11">
         <v>15</v>
       </c>
-      <c r="T25" s="23">
+      <c r="T25" s="11">
         <v>7.1</v>
       </c>
     </row>
-    <row r="26" spans="2:20" s="28" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="31">
+    <row r="26" spans="2:20" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="30">
         <v>45107</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="8">
         <v>5.6</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="8">
         <v>5.7</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="8">
         <v>5.4</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="8">
         <v>18.5</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="8">
         <v>15.1</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="8">
         <v>23.4</v>
       </c>
-      <c r="I26" s="21">
+      <c r="I26" s="9">
         <v>12.9</v>
       </c>
-      <c r="J26" s="21">
+      <c r="J26" s="9">
         <v>9.3999999999999986</v>
       </c>
-      <c r="K26" s="21">
+      <c r="K26" s="9">
         <v>18</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="10">
         <v>4.7</v>
       </c>
-      <c r="M26" s="22">
+      <c r="M26" s="10">
         <v>3.2</v>
       </c>
-      <c r="N26" s="22">
+      <c r="N26" s="10">
         <v>5.2</v>
       </c>
-      <c r="O26" s="22">
+      <c r="O26" s="10">
         <v>13.7</v>
       </c>
-      <c r="P26" s="22">
+      <c r="P26" s="10">
         <v>14.4</v>
       </c>
-      <c r="Q26" s="22">
+      <c r="Q26" s="10">
         <v>13.5</v>
       </c>
-      <c r="R26" s="23">
+      <c r="R26" s="11">
         <v>9</v>
       </c>
-      <c r="S26" s="23">
+      <c r="S26" s="11">
         <v>11.2</v>
       </c>
-      <c r="T26" s="23">
+      <c r="T26" s="11">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-    </row>
-    <row r="28" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="32" t="s">
+    <row r="27" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+    </row>
+    <row r="28" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="13"/>
+    </row>
+    <row r="30" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
-    </row>
-    <row r="30" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="26" t="s">
+    <row r="32" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="26" t="s">
+    <row r="33" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="2:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="27" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="R6:T6"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="L8:Q8"/>
     <mergeCell ref="R8:T8"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
     <mergeCell ref="L6:N6"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>